<commit_message>
Add extra query button, display google result, fix layout
</commit_message>
<xml_diff>
--- a/emma/Insert Multi Rows QUERY.xlsx
+++ b/emma/Insert Multi Rows QUERY.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="47">
   <si>
     <t>test_user</t>
   </si>
@@ -129,6 +130,42 @@
   </si>
   <si>
     <t>how tall is michelle obama</t>
+  </si>
+  <si>
+    <t>Hi John, Michael Jordan is 1.98 metres tall.</t>
+  </si>
+  <si>
+    <t>Hi John, Barack Obama is 1.85 metres tall.</t>
+  </si>
+  <si>
+    <t>queryid</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>2016-04-11 09:30:00</t>
+  </si>
+  <si>
+    <t>2016-04-11 09:31:00</t>
   </si>
 </sst>
 </file>
@@ -460,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,24 +544,24 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
-        <v>7</v>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="L1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M1" t="str">
-        <f>"INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES ("</f>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <f>"INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES ("</f>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N1" t="str">
-        <f>M1 &amp; A1 &amp; ",'" &amp; B1 &amp; "','" &amp; C1 &amp; "','" &amp; D1 &amp; "'," &amp; E1 &amp; ",'" &amp; F1 &amp; "','" &amp; G1 &amp; "','" &amp; H1 &amp; "'," &amp; I1 &amp; ",'" &amp; J1 &amp; "'," &amp; K1 &amp; "," &amp; L1 &amp; ");"</f>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (1,'test_user','2016-04-11 09:00:00','-33.7687822,150.904814',1,'how tall is michael jordan','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <f>M1 &amp; A1 &amp; ",'" &amp; B1 &amp; "','" &amp; C1 &amp; "','" &amp; D1 &amp; "'," &amp; E1 &amp; ",'" &amp; F1 &amp; "','" &amp; G1 &amp; "','" &amp; H1 &amp; "','" &amp; I1 &amp; "','" &amp; J1 &amp; "','" &amp; K1 &amp; "'," &amp; L1 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (1,'test_user','2016-04-11 09:00:00','-33.7687822,150.904814',1,'how tall is michael jordan','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','Hi John, Michael Jordan is 1.98 metres tall.','test_agent','2016-04-11 09:00:00',2);</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -553,24 +590,24 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
-        <v>7</v>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M10" si="0">"INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES ("</f>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <f t="shared" ref="M2:M10" si="0">"INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES ("</f>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N2" t="str">
-        <f t="shared" ref="N2:N10" si="1">M2 &amp; A2 &amp; ",'" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "'," &amp; E2 &amp; ",'" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "'," &amp; I2 &amp; ",'" &amp; J2 &amp; "'," &amp; K2 &amp; "," &amp; L2 &amp; ");"</f>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (2,'test_user','2016-04-11 09:00:01','-33.7687822,150.904815',1,'how tall is barack obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <f>M2 &amp; A2 &amp; ",'" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "'," &amp; E2 &amp; ",'" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','" &amp; I2 &amp; "','" &amp; J2 &amp; "','" &amp; K2 &amp; "'," &amp; L2 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (2,'test_user','2016-04-11 09:00:01','-33.7687822,150.904815',1,'how tall is barack obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','Hi John, Barack Obama is 1.85 metres tall.','test_agent','2016-04-11 09:00:00',2);</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -602,9 +639,9 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L3">
@@ -612,11 +649,11 @@
       </c>
       <c r="M3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (3,'test_user','2016-04-11 09:00:02','-33.7687822,150.904816',1,'how tall is hilary clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <f>M3 &amp; A3 &amp; ",'" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "'," &amp; E3 &amp; ",'" &amp; F3 &amp; "','" &amp; G3 &amp; "','" &amp; H3 &amp; "'," &amp; I3 &amp; "," &amp; J3 &amp; "," &amp; K3 &amp; "," &amp; L3 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (3,'test_user','2016-04-11 09:00:02','-33.7687822,150.904816',1,'how tall is hilary clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -648,7 +685,7 @@
         <v>7</v>
       </c>
       <c r="J4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K4" t="s">
         <v>7</v>
@@ -658,11 +695,11 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (4,'test_user','2016-04-11 09:00:03','-33.7687822,150.904817',1,'how tall is napolean bonaparte','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <f t="shared" ref="N4:N10" si="1">M4 &amp; A4 &amp; ",'" &amp; B4 &amp; "','" &amp; C4 &amp; "','" &amp; D4 &amp; "'," &amp; E4 &amp; ",'" &amp; F4 &amp; "','" &amp; G4 &amp; "','" &amp; H4 &amp; "'," &amp; I4 &amp; "," &amp; J4 &amp; "," &amp; K4 &amp; "," &amp; L4 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (4,'test_user','2016-04-11 09:00:03','-33.7687822,150.904817',1,'how tall is napolean bonaparte','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -694,7 +731,7 @@
         <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K5" t="s">
         <v>7</v>
@@ -704,11 +741,11 @@
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (5,'test_user','2016-04-11 09:00:04','-33.7687822,150.904818',1,'how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (5,'test_user','2016-04-11 09:00:04','-33.7687822,150.904818',1,'how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -740,7 +777,7 @@
         <v>7</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K6" t="s">
         <v>7</v>
@@ -750,11 +787,11 @@
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (6,'test_user','2016-04-11 09:00:05','-33.7687822,150.904819',1,'how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (6,'test_user','2016-04-11 09:00:05','-33.7687822,150.904819',1,'how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -786,7 +823,7 @@
         <v>7</v>
       </c>
       <c r="J7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K7" t="s">
         <v>7</v>
@@ -796,11 +833,11 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (7,'test_user','2016-04-11 09:00:06','-33.7687822,150.904820',1,'how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (7,'test_user','2016-04-11 09:00:06','-33.7687822,150.904820',1,'how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -832,7 +869,7 @@
         <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K8" t="s">
         <v>7</v>
@@ -842,11 +879,11 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (8,'test_user','2016-04-11 09:00:07','-33.7687822,150.904821',1,'how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (8,'test_user','2016-04-11 09:00:07','-33.7687822,150.904821',1,'how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -878,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="J9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K9" t="s">
         <v>7</v>
@@ -888,11 +925,11 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (9,'test_user','2016-04-11 09:00:08','-33.7687822,150.904822',1,'how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (9,'test_user','2016-04-11 09:00:08','-33.7687822,150.904822',1,'how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -924,7 +961,7 @@
         <v>7</v>
       </c>
       <c r="J10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K10" t="s">
         <v>7</v>
@@ -934,11 +971,11 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO QUERY (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (10,'test_user','2016-04-11 09:00:09','-33.7687822,150.904823',1,'how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,'test_agent',NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, type, content, audio, image, answer, answeredby, answertime, status) VALUES (10,'test_user','2016-04-11 09:00:09','-33.7687822,150.904823',1,'how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
   </sheetData>
@@ -959,4 +996,348 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId5"/>
+    <hyperlink ref="H6" r:id="rId6"/>
+    <hyperlink ref="H7" r:id="rId7"/>
+    <hyperlink ref="H8" r:id="rId8"/>
+    <hyperlink ref="H9" r:id="rId9"/>
+    <hyperlink ref="H10" r:id="rId10"/>
+    <hyperlink ref="H11" r:id="rId11"/>
+    <hyperlink ref="G3:G11" r:id="rId12" display="http://www.soundjay.com/misc/bell-ringing-01.mp3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>